<commit_message>
feitas modificações na folha excel com resultados dos testes
</commit_message>
<xml_diff>
--- a/testes.xlsx
+++ b/testes.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Documents\GitHub\lei\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Google Drive\universidade\LEI\lei\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142D31CC-BA82-43A3-9FED-CC2F6D372E3C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exp. maquinas" sheetId="6" r:id="rId1"/>
     <sheet name="grafico" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,19 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
-  <si>
-    <t>media</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>n pedidos</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Processador</t>
   </si>
@@ -60,13 +49,31 @@
     <t>ubuntu 16.04.4 64bits</t>
   </si>
   <si>
-    <t>tempo total(s)</t>
+    <t>min(ms)</t>
+  </si>
+  <si>
+    <t>max(ms)</t>
+  </si>
+  <si>
+    <t>Métricas por pedido</t>
+  </si>
+  <si>
+    <t>Tempo total de execução de todos os pedidos (s)</t>
+  </si>
+  <si>
+    <t>Nível de concorrência</t>
+  </si>
+  <si>
+    <t>1 milhão de pedidos em cada teste</t>
+  </si>
+  <si>
+    <t>média(ms)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -84,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -107,11 +114,140 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -123,6 +259,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -175,11 +346,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>grafico!$D$3</c:f>
+              <c:f>grafico!$D$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>media</c:v>
+                  <c:v>média(ms)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -198,7 +369,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>grafico!$B$4:$B$15</c:f>
+              <c:f>grafico!$B$9:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -243,7 +414,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>grafico!$D$4:$D$15</c:f>
+              <c:f>grafico!$D$9:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -290,6 +461,131 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-EF27-4AC5-8C6F-061967E46BAE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>grafico!$G$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tempo total de execução de todos os pedidos (s)</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>grafico!$B$9:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>grafico!$G$9:$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>657</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>363</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>293</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>283</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>388</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-EF27-4AC5-8C6F-061967E46BAE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -315,14 +611,14 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>grafico!$C$3</c15:sqref>
+                          <c15:sqref>grafico!$C$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>min</c:v>
+                        <c:v>min(ms)</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -344,7 +640,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>grafico!$B$4:$B$15</c15:sqref>
+                          <c15:sqref>grafico!$B$9:$B$20</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -395,7 +691,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>grafico!$C$4:$C$15</c15:sqref>
+                          <c15:sqref>grafico!$C$9:$C$20</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -455,17 +751,17 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>grafico!$E$3</c15:sqref>
+                          <c15:sqref>grafico!$E$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>max</c:v>
+                        <c:v>max(ms)</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -484,10 +780,10 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>grafico!$B$4:$B$15</c15:sqref>
+                          <c15:sqref>grafico!$B$9:$B$20</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -535,10 +831,10 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>grafico!$E$4:$E$15</c15:sqref>
+                          <c15:sqref>grafico!$E$9:$E$20</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -585,143 +881,9 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-EF27-4AC5-8C6F-061967E46BAE}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="4"/>
-                <c:order val="3"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>grafico!$F$3</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>tempo total(s)</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="none"/>
-                </c:marker>
-                <c:cat>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>grafico!$B$4:$B$15</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="12"/>
-                      <c:pt idx="0">
-                        <c:v>1</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>2</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>4</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>8</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>16</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>32</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>64</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>128</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>256</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>512</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>800</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>1000</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:cat>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>grafico!$F$4:$F$12</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="9"/>
-                      <c:pt idx="0">
-                        <c:v>657</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>2754</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>3410</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>283</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>258</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>253</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>313</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>240</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>209</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000004-EF27-4AC5-8C6F-061967E46BAE}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -1472,16 +1634,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>610913</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>2956</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1805,7 +1967,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1825,39 +1987,39 @@
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="3:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="3:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="3:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1866,248 +2028,281 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>1000000</v>
-      </c>
+    <row r="2" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="5" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="12">
+        <v>1</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0</v>
+      </c>
+      <c r="D9" s="14">
+        <v>0</v>
+      </c>
+      <c r="E9" s="14">
+        <v>20</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="10">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C10" s="16">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D10" s="17">
+        <v>0</v>
+      </c>
+      <c r="E10" s="17">
+        <v>54</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="10">
+        <v>4</v>
+      </c>
+      <c r="C11" s="16">
+        <v>0</v>
+      </c>
+      <c r="D11" s="17">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
+      <c r="E11" s="17">
+        <v>202</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18">
+        <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
+        <v>8</v>
+      </c>
+      <c r="C12" s="16">
+        <v>0</v>
+      </c>
+      <c r="D12" s="17">
+        <v>2</v>
+      </c>
+      <c r="E12" s="17">
+        <v>3855</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="10">
+        <v>16</v>
+      </c>
+      <c r="C13" s="16">
+        <v>0</v>
+      </c>
+      <c r="D13" s="17">
+        <v>4</v>
+      </c>
+      <c r="E13" s="17">
+        <v>587</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="10">
+        <v>32</v>
+      </c>
+      <c r="C14" s="16">
+        <v>0</v>
+      </c>
+      <c r="D14" s="17">
+        <v>8</v>
+      </c>
+      <c r="E14" s="17">
+        <v>3956</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="18">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="21">
+        <v>64</v>
+      </c>
+      <c r="C15" s="17">
+        <v>0</v>
+      </c>
+      <c r="D15" s="17">
+        <v>20</v>
+      </c>
+      <c r="E15" s="17">
+        <v>7017</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="19">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="10">
+        <v>128</v>
+      </c>
+      <c r="C16" s="16">
+        <v>0</v>
+      </c>
+      <c r="D16" s="17">
+        <v>30</v>
+      </c>
+      <c r="E16" s="17">
+        <v>7024</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="18">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="10">
+        <v>256</v>
+      </c>
+      <c r="C17" s="16">
+        <v>0</v>
+      </c>
+      <c r="D17" s="17">
+        <v>53</v>
+      </c>
+      <c r="E17" s="17">
+        <v>15041</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="10">
+        <v>512</v>
+      </c>
+      <c r="C18" s="16">
+        <v>0</v>
+      </c>
+      <c r="D18" s="17">
+        <v>156</v>
+      </c>
+      <c r="E18" s="17">
+        <v>28242</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="18">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="10">
+        <v>800</v>
+      </c>
+      <c r="C19" s="16">
         <v>1</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>20</v>
-      </c>
-      <c r="F4">
-        <v>657</v>
+      <c r="D19" s="17">
+        <v>309</v>
+      </c>
+      <c r="E19" s="17">
+        <v>18272</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18">
+        <v>388</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>54</v>
-      </c>
-      <c r="F5">
-        <v>2754</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="10">
+        <v>1000</v>
+      </c>
+      <c r="C20" s="16">
         <v>1</v>
       </c>
-      <c r="E6">
-        <v>202</v>
-      </c>
-      <c r="F6">
-        <v>3410</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>3855</v>
-      </c>
-      <c r="F7">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>16</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
-      <c r="E8">
-        <v>587</v>
-      </c>
-      <c r="F8">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>32</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
-      <c r="E9">
-        <v>3956</v>
-      </c>
-      <c r="F9">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>64</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>20</v>
-      </c>
-      <c r="E10">
-        <v>7017</v>
-      </c>
-      <c r="F10">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>128</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>30</v>
-      </c>
-      <c r="E11">
-        <v>7024</v>
-      </c>
-      <c r="F11">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>256</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>53</v>
-      </c>
-      <c r="E12">
-        <v>15041</v>
-      </c>
-      <c r="F12">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>512</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>156</v>
-      </c>
-      <c r="E13">
-        <v>28242</v>
-      </c>
-      <c r="F13">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>800</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>309</v>
-      </c>
-      <c r="E14">
-        <v>18272</v>
-      </c>
-      <c r="F14">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>1000</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
+      <c r="D20" s="17">
         <v>214</v>
       </c>
-      <c r="E15">
+      <c r="E20" s="17">
         <v>31078</v>
       </c>
-      <c r="F15">
+      <c r="F20" s="17"/>
+      <c r="G20" s="18">
         <v>216</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="B4:D4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>